<commit_message>
developing processing and testing
</commit_message>
<xml_diff>
--- a/latlong-processing/src/Data/analise.xlsx
+++ b/latlong-processing/src/Data/analise.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projetos\paulo3011\spark-processing-samples\latlong-processing\src\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94A07A2-6550-4EC7-A7AA-7B688439F30C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA45E9A-8E28-4CCE-B91F-70E1F3D64319}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0D960920-D906-47EC-8442-17DC1C46953B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{0D960920-D906-47EC-8442-17DC1C46953B}"/>
   </bookViews>
   <sheets>
     <sheet name="posicoes_tratado" sheetId="3" r:id="rId1"/>
-    <sheet name="Planilha1" sheetId="1" r:id="rId2"/>
+    <sheet name="tempo_total_frota" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="DadosExternos_1" localSheetId="0" hidden="1">posicoes_tratado!$A$1:$F$929</definedName>
@@ -10880,7 +10880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{997F37A1-196B-480C-A3B5-4C39464FA881}">
   <dimension ref="A1:M930"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I801" sqref="I801"/>
     </sheetView>
   </sheetViews>
@@ -40747,7 +40747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95F9DFA-7E5E-45B1-9A62-52BF31F6F8A3}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>